<commit_message>
finished data showing counts after second round
</commit_message>
<xml_diff>
--- a/Book Package Optimization Example.xlsx
+++ b/Book Package Optimization Example.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mando\Projects\unfoldingWord\book-package-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CE137A-B772-4636-8D9B-6B25162F772E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377F51A6-EE2E-4BE5-84A6-FFE014493194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{0F2DA732-D3F7-40CE-BD5C-6DEBF124DB21}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{0F2DA732-D3F7-40CE-BD5C-6DEBF124DB21}"/>
   </bookViews>
   <sheets>
-    <sheet name="Optimization" sheetId="1" r:id="rId1"/>
+    <sheet name="Round 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Round 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="146">
   <si>
     <t>rc://*/tw/dict/bible/kt/antichrist</t>
   </si>
@@ -468,6 +469,9 @@
   </si>
   <si>
     <t>3 John Total without 2JN articles</t>
+  </si>
+  <si>
+    <t>1 John Total without 2JN or 3JN articles</t>
   </si>
 </sst>
 </file>
@@ -537,16 +541,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -639,6 +643,78 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -662,6 +738,24 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -676,7 +770,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{048F78AD-08F4-45F8-9F84-020BE237E3E4}" name="Table1" displayName="Table1" ref="A2:D47" totalsRowCount="1" headerRowDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{048F78AD-08F4-45F8-9F84-020BE237E3E4}" name="Table1" displayName="Table1" ref="A2:D47" totalsRowCount="1" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A2:D46" xr:uid="{61F6623E-FEE4-4A4C-AF10-FE0384432798}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{FE2A1EBB-C49D-4626-8398-C580855A6565}" name="Article"/>
@@ -691,7 +785,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A7B3CF0-9D75-4FBA-9C16-B377CE4EDFDB}" name="Table2" displayName="Table2" ref="F2:I46" totalsRowCount="1" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A7B3CF0-9D75-4FBA-9C16-B377CE4EDFDB}" name="Table2" displayName="Table2" ref="F2:I46" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="F2:I45" xr:uid="{B73A5317-C690-46AE-A395-1F7B3C37F92F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9E0CD048-5002-4771-85D3-983995F6B0FE}" name="Article"/>
@@ -706,15 +800,45 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0672DA39-0B60-4E55-8CA6-4712701F3938}" name="Table3" displayName="Table3" ref="K2:N111" totalsRowCount="1" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0672DA39-0B60-4E55-8CA6-4712701F3938}" name="Table3" displayName="Table3" ref="K2:N111" totalsRowCount="1" headerRowDxfId="8">
   <autoFilter ref="K2:N110" xr:uid="{8F94B494-4B3D-43CF-A92E-0BEC661DC4E9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F88C3759-9B82-4887-BFC4-E1BD0CF7848C}" name="Article"/>
-    <tableColumn id="2" xr3:uid="{AAB3A2DE-B542-47E6-9A08-B474DC7BFD06}" name="Ref count" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8AF989D8-F58C-4632-8184-D0D8EB167D89}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="1">
+    <tableColumn id="2" xr3:uid="{AAB3A2DE-B542-47E6-9A08-B474DC7BFD06}" name="Ref count" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{8AF989D8-F58C-4632-8184-D0D8EB167D89}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Table3[Word Count])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A47B8975-32CE-43A0-B699-CC4E6C9EFB29}" name="Unique Words" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{A47B8975-32CE-43A0-B699-CC4E6C9EFB29}" name="Unique Words" totalsRowDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E578C125-48CC-4665-9723-267CC4102C28}" name="Table25" displayName="Table25" ref="A2:D46" totalsRowCount="1" headerRowDxfId="4">
+  <autoFilter ref="A2:D45" xr:uid="{285EC3D1-0938-4CF9-9BC4-DC3F03A96066}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B38042D9-2789-456B-90B0-E3F19FB8CFEE}" name="Article"/>
+    <tableColumn id="2" xr3:uid="{402ED6FB-EA13-4F5B-BF59-E93C6BDAE936}" name="Ref Count"/>
+    <tableColumn id="3" xr3:uid="{EB2CE401-08B0-48EC-B558-2D758489B37F}" name="Word Count" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table25[Word Count])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{FF0E3C5F-34F5-4CED-BDCB-488DA8A5307B}" name="Unique Words"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{93D4F411-94F7-4A13-91B4-AD636EA4BC08}" name="Table36" displayName="Table36" ref="F2:I111" totalsRowCount="1" headerRowDxfId="3">
+  <autoFilter ref="F2:I110" xr:uid="{B6F971C8-6BBC-4A3A-A96F-181A54505C10}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{21266393-F363-42BC-BF78-77C9A73987F9}" name="Article"/>
+    <tableColumn id="2" xr3:uid="{19B656FE-C087-43E5-A2F0-47A162F52579}" name="Ref count" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8B18F271-2A76-402A-AD3E-AB1C3D626820}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="1">
+      <totalsRowFormula>SUM(Table36[Word Count])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{3C9FC25C-592E-42BB-AEA2-DB3562835A34}" name="Unique Words" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1019,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB18D55C-4F58-498B-85D4-1490E4DDD645}">
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="M114" sqref="M114"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,12 +1153,12 @@
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="35.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="3.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" style="2" customWidth="1"/>
@@ -1042,24 +1166,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1074,7 +1198,7 @@
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1087,7 +1211,7 @@
       <c r="I2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="3"/>
       <c r="K2" t="s">
         <v>37</v>
       </c>
@@ -3924,4 +4048,2164 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E514ECA4-E30C-4BE7-995D-7555FADB58D2}">
+  <dimension ref="A1:I114"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="H114" sqref="H114"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>160</v>
+      </c>
+      <c r="D3">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>314</v>
+      </c>
+      <c r="I3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>338</v>
+      </c>
+      <c r="D4">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>171</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>728</v>
+      </c>
+      <c r="I5">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>367</v>
+      </c>
+      <c r="D6">
+        <v>157</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>243</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>337</v>
+      </c>
+      <c r="I7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>461</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>248</v>
+      </c>
+      <c r="I8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>143</v>
+      </c>
+      <c r="D9">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>255</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>483</v>
+      </c>
+      <c r="I10">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>520</v>
+      </c>
+      <c r="D11">
+        <v>270</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>136</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>291</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>469</v>
+      </c>
+      <c r="I13">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>292</v>
+      </c>
+      <c r="D14">
+        <v>124</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>323</v>
+      </c>
+      <c r="D15">
+        <v>173</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>134</v>
+      </c>
+      <c r="I15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>175</v>
+      </c>
+      <c r="D16">
+        <v>91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>648</v>
+      </c>
+      <c r="D17">
+        <v>220</v>
+      </c>
+      <c r="F17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>462</v>
+      </c>
+      <c r="I17">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>184</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>110</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>367</v>
+      </c>
+      <c r="I19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>230</v>
+      </c>
+      <c r="D20">
+        <v>87</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>133</v>
+      </c>
+      <c r="D21">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>481</v>
+      </c>
+      <c r="I21">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>109</v>
+      </c>
+      <c r="D22">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>224</v>
+      </c>
+      <c r="I22">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>143</v>
+      </c>
+      <c r="I23">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>410</v>
+      </c>
+      <c r="D24">
+        <v>225</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>138</v>
+      </c>
+      <c r="D25">
+        <v>78</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>385</v>
+      </c>
+      <c r="I25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>193</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>62</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>140</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>297</v>
+      </c>
+      <c r="I28">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>144</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>412</v>
+      </c>
+      <c r="I29">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>155</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>239</v>
+      </c>
+      <c r="D31">
+        <v>132</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>139</v>
+      </c>
+      <c r="I31">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>172</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <v>12</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>219</v>
+      </c>
+      <c r="D33">
+        <v>135</v>
+      </c>
+      <c r="F33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>387</v>
+      </c>
+      <c r="I33">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34">
+        <v>17</v>
+      </c>
+      <c r="H34">
+        <v>455</v>
+      </c>
+      <c r="I34">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>902</v>
+      </c>
+      <c r="D35">
+        <v>206</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35">
+        <v>46</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>803</v>
+      </c>
+      <c r="D36">
+        <v>211</v>
+      </c>
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>480</v>
+      </c>
+      <c r="D37">
+        <v>173</v>
+      </c>
+      <c r="F37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1555</v>
+      </c>
+      <c r="D38">
+        <v>297</v>
+      </c>
+      <c r="F38" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>290</v>
+      </c>
+      <c r="I38">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>239</v>
+      </c>
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>118</v>
+      </c>
+      <c r="I39">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>441</v>
+      </c>
+      <c r="D40">
+        <v>169</v>
+      </c>
+      <c r="F40" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>280</v>
+      </c>
+      <c r="I40">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>594</v>
+      </c>
+      <c r="F41" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <v>201</v>
+      </c>
+      <c r="I41">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>175</v>
+      </c>
+      <c r="F42" t="s">
+        <v>95</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>593</v>
+      </c>
+      <c r="I42">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>566</v>
+      </c>
+      <c r="D43">
+        <v>201</v>
+      </c>
+      <c r="F43" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43">
+        <v>9</v>
+      </c>
+      <c r="H43">
+        <v>435</v>
+      </c>
+      <c r="I43">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>85</v>
+      </c>
+      <c r="F44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>162</v>
+      </c>
+      <c r="I44">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>1398</v>
+      </c>
+      <c r="D45">
+        <v>276</v>
+      </c>
+      <c r="F45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45">
+        <v>27</v>
+      </c>
+      <c r="H45">
+        <v>600</v>
+      </c>
+      <c r="I45">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f>SUM(Table25[Word Count])</f>
+        <v>11050</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46">
+        <v>22</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47">
+        <f>10206+10509</f>
+        <v>20715</v>
+      </c>
+      <c r="F47" t="s">
+        <v>99</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="H47">
+        <v>467</v>
+      </c>
+      <c r="I47">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48">
+        <f>C47-Table25[[#Totals],[Word Count]]</f>
+        <v>9665</v>
+      </c>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>281</v>
+      </c>
+      <c r="I48">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49">
+        <f>22903-C48</f>
+        <v>13238</v>
+      </c>
+      <c r="F49" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49">
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>16</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>101</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>98</v>
+      </c>
+      <c r="I51">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>102</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>570</v>
+      </c>
+      <c r="I52">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54">
+        <v>23</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>103</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>112</v>
+      </c>
+      <c r="I55">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>104</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>171</v>
+      </c>
+      <c r="I57">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>105</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>164</v>
+      </c>
+      <c r="I58">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>106</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>114</v>
+      </c>
+      <c r="I59">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>159</v>
+      </c>
+      <c r="I60">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>108</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <v>188</v>
+      </c>
+      <c r="I61">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62">
+        <v>4</v>
+      </c>
+      <c r="H62">
+        <v>223</v>
+      </c>
+      <c r="I62">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>110</v>
+      </c>
+      <c r="G63">
+        <v>7</v>
+      </c>
+      <c r="H63">
+        <v>260</v>
+      </c>
+      <c r="I63">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>111</v>
+      </c>
+      <c r="G64">
+        <v>6</v>
+      </c>
+      <c r="H64">
+        <v>527</v>
+      </c>
+      <c r="I64">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>112</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <v>195</v>
+      </c>
+      <c r="I66">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>113</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>107</v>
+      </c>
+      <c r="I67">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>114</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>271</v>
+      </c>
+      <c r="I68">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>115</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>465</v>
+      </c>
+      <c r="I69">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="70" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>116</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>200</v>
+      </c>
+      <c r="I70">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72">
+        <v>40</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>117</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="H73">
+        <v>510</v>
+      </c>
+      <c r="I73">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>118</v>
+      </c>
+      <c r="G74">
+        <v>6</v>
+      </c>
+      <c r="H74">
+        <v>289</v>
+      </c>
+      <c r="I74">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75">
+        <v>12</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>119</v>
+      </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
+      <c r="H76">
+        <v>132</v>
+      </c>
+      <c r="I76">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>120</v>
+      </c>
+      <c r="G77">
+        <v>7</v>
+      </c>
+      <c r="H77">
+        <v>265</v>
+      </c>
+      <c r="I77">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>121</v>
+      </c>
+      <c r="G78">
+        <v>5</v>
+      </c>
+      <c r="H78">
+        <v>147</v>
+      </c>
+      <c r="I78">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>122</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>373</v>
+      </c>
+      <c r="I79">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>31</v>
+      </c>
+      <c r="G80">
+        <v>3</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>123</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>277</v>
+      </c>
+      <c r="I81">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>65</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>124</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>127</v>
+      </c>
+      <c r="I83">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>125</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>409</v>
+      </c>
+      <c r="I84">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>126</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>174</v>
+      </c>
+      <c r="I85">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>34</v>
+      </c>
+      <c r="G86">
+        <v>3</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>127</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>216</v>
+      </c>
+      <c r="I87">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>128</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>143</v>
+      </c>
+      <c r="I88">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>35</v>
+      </c>
+      <c r="G89">
+        <v>5</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>129</v>
+      </c>
+      <c r="G90">
+        <v>4</v>
+      </c>
+      <c r="H90">
+        <v>342</v>
+      </c>
+      <c r="I90">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>130</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>125</v>
+      </c>
+      <c r="I91">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>131</v>
+      </c>
+      <c r="G92">
+        <v>7</v>
+      </c>
+      <c r="H92">
+        <v>807</v>
+      </c>
+      <c r="I92">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="93" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>66</v>
+      </c>
+      <c r="G93">
+        <v>12</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="94" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>132</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+      <c r="H94">
+        <v>775</v>
+      </c>
+      <c r="I94">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>133</v>
+      </c>
+      <c r="G95">
+        <v>2</v>
+      </c>
+      <c r="H95">
+        <v>487</v>
+      </c>
+      <c r="I95">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="96" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>67</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>68</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>42</v>
+      </c>
+      <c r="G98">
+        <v>6</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>134</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1396</v>
+      </c>
+      <c r="I99">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>44</v>
+      </c>
+      <c r="G100">
+        <v>3</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="101" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>69</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="102" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
+        <v>45</v>
+      </c>
+      <c r="G102">
+        <v>50</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="103" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>46</v>
+      </c>
+      <c r="G103">
+        <v>28</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="104" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F104" t="s">
+        <v>135</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+      <c r="H104">
+        <v>916</v>
+      </c>
+      <c r="I104">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="105" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G105">
+        <v>2</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="106" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>136</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="H106">
+        <v>1018</v>
+      </c>
+      <c r="I106">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="107" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>137</v>
+      </c>
+      <c r="G107">
+        <v>4</v>
+      </c>
+      <c r="H107">
+        <v>1376</v>
+      </c>
+      <c r="I107">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="108" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
+        <v>138</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="H108">
+        <v>344</v>
+      </c>
+      <c r="I108">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>47</v>
+      </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="110" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>48</v>
+      </c>
+      <c r="G110">
+        <v>12</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="111" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H111" s="2">
+        <f>SUM(Table36[Word Count])</f>
+        <v>24364</v>
+      </c>
+    </row>
+    <row r="112" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
+        <v>142</v>
+      </c>
+      <c r="H112" s="2">
+        <f>27986+16932</f>
+        <v>44918</v>
+      </c>
+    </row>
+    <row r="113" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>141</v>
+      </c>
+      <c r="H113" s="2">
+        <f>H112-Table36[[#Totals],[Word Count]]</f>
+        <v>20554</v>
+      </c>
+    </row>
+    <row r="114" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>145</v>
+      </c>
+      <c r="H114" s="2">
+        <f>61135-H113</f>
+        <v>40581</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing of optimization results and fixes
</commit_message>
<xml_diff>
--- a/Book Package Optimization Example.xlsx
+++ b/Book Package Optimization Example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mando\Projects\unfoldingWord\book-package-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377F51A6-EE2E-4BE5-84A6-FFE014493194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58409BA8-99D7-4E20-A012-88F823A11531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{0F2DA732-D3F7-40CE-BD5C-6DEBF124DB21}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="147">
   <si>
     <t>rc://*/tw/dict/bible/kt/antichrist</t>
   </si>
@@ -465,13 +465,16 @@
     <t>Total article word count with all articles</t>
   </si>
   <si>
-    <t>1 John Total without 2JN articles</t>
-  </si>
-  <si>
     <t>3 John Total without 2JN articles</t>
   </si>
   <si>
-    <t>1 John Total without 2JN or 3JN articles</t>
+    <t>Book Total Word Count</t>
+  </si>
+  <si>
+    <t>book oriented total (ULT, UST, UTQ, UTN)</t>
+  </si>
+  <si>
+    <t>3 John Total without 1JN and 2JN articles</t>
   </si>
 </sst>
 </file>
@@ -607,25 +610,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -679,7 +664,25 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -804,18 +807,18 @@
   <autoFilter ref="K2:N110" xr:uid="{8F94B494-4B3D-43CF-A92E-0BEC661DC4E9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F88C3759-9B82-4887-BFC4-E1BD0CF7848C}" name="Article"/>
-    <tableColumn id="2" xr3:uid="{AAB3A2DE-B542-47E6-9A08-B474DC7BFD06}" name="Ref count" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{8AF989D8-F58C-4632-8184-D0D8EB167D89}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="6">
+    <tableColumn id="2" xr3:uid="{AAB3A2DE-B542-47E6-9A08-B474DC7BFD06}" name="Ref count" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8AF989D8-F58C-4632-8184-D0D8EB167D89}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="1">
       <totalsRowFormula>SUM(Table3[Word Count])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A47B8975-32CE-43A0-B699-CC4E6C9EFB29}" name="Unique Words" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A47B8975-32CE-43A0-B699-CC4E6C9EFB29}" name="Unique Words" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E578C125-48CC-4665-9723-267CC4102C28}" name="Table25" displayName="Table25" ref="A2:D46" totalsRowCount="1" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E578C125-48CC-4665-9723-267CC4102C28}" name="Table25" displayName="Table25" ref="A2:D46" totalsRowCount="1" headerRowDxfId="7">
   <autoFilter ref="A2:D45" xr:uid="{285EC3D1-0938-4CF9-9BC4-DC3F03A96066}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B38042D9-2789-456B-90B0-E3F19FB8CFEE}" name="Article"/>
@@ -830,15 +833,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{93D4F411-94F7-4A13-91B4-AD636EA4BC08}" name="Table36" displayName="Table36" ref="F2:I111" totalsRowCount="1" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{93D4F411-94F7-4A13-91B4-AD636EA4BC08}" name="Table36" displayName="Table36" ref="F2:I111" totalsRowCount="1" headerRowDxfId="6">
   <autoFilter ref="F2:I110" xr:uid="{B6F971C8-6BBC-4A3A-A96F-181A54505C10}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{21266393-F363-42BC-BF78-77C9A73987F9}" name="Article"/>
-    <tableColumn id="2" xr3:uid="{19B656FE-C087-43E5-A2F0-47A162F52579}" name="Ref count" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{8B18F271-2A76-402A-AD3E-AB1C3D626820}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="1">
+    <tableColumn id="2" xr3:uid="{19B656FE-C087-43E5-A2F0-47A162F52579}" name="Ref count" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8B18F271-2A76-402A-AD3E-AB1C3D626820}" name="Word Count" totalsRowFunction="custom" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Table36[Word Count])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3C9FC25C-592E-42BB-AEA2-DB3562835A34}" name="Unique Words" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3C9FC25C-592E-42BB-AEA2-DB3562835A34}" name="Unique Words" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1141,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB18D55C-4F58-498B-85D4-1490E4DDD645}">
-  <dimension ref="A1:N114"/>
+  <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="K114" sqref="K114:M115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,7 +2578,7 @@
         <v>1</v>
       </c>
       <c r="H38">
-        <v>1555</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <v>297</v>
@@ -2874,7 +2877,7 @@
       </c>
       <c r="H46">
         <f>SUM(Table2[Word Count])</f>
-        <v>11050</v>
+        <v>9495</v>
       </c>
       <c r="K46" t="s">
         <v>16</v>
@@ -2917,15 +2920,20 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
       <c r="B48"/>
-      <c r="C48"/>
+      <c r="C48">
+        <v>20668</v>
+      </c>
       <c r="D48"/>
       <c r="F48" t="s">
         <v>141</v>
       </c>
       <c r="H48">
         <f>H47-Table2[[#Totals],[Word Count]]</f>
-        <v>9665</v>
+        <v>11220</v>
       </c>
       <c r="K48" t="s">
         <v>100</v>
@@ -2948,8 +2956,7 @@
         <v>144</v>
       </c>
       <c r="H49">
-        <f>22903-H48</f>
-        <v>13238</v>
+        <v>22903</v>
       </c>
       <c r="K49" t="s">
         <v>58</v>
@@ -2968,6 +2975,13 @@
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
+      <c r="F50" t="s">
+        <v>143</v>
+      </c>
+      <c r="H50">
+        <f>H49-H48</f>
+        <v>11683</v>
+      </c>
       <c r="K50" t="s">
         <v>18</v>
       </c>
@@ -3026,7 +3040,7 @@
         <v>3</v>
       </c>
       <c r="M53">
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="N53">
         <v>110</v>
@@ -4004,7 +4018,7 @@
     <row r="111" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M111" s="2">
         <f>SUM(Table3[Word Count])</f>
-        <v>30257</v>
+        <v>29997</v>
       </c>
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.25">
@@ -4016,22 +4030,54 @@
         <v>44918</v>
       </c>
     </row>
-    <row r="113" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K113" t="s">
         <v>141</v>
       </c>
       <c r="M113" s="2">
         <f>M112-Table3[[#Totals],[Word Count]]</f>
-        <v>14661</v>
-      </c>
-    </row>
-    <row r="114" spans="11:13" x14ac:dyDescent="0.25">
+        <v>14921</v>
+      </c>
+    </row>
+    <row r="114" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K114" t="s">
+        <v>144</v>
+      </c>
+      <c r="M114" s="2">
+        <v>61135</v>
+      </c>
+    </row>
+    <row r="115" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K115" t="s">
         <v>143</v>
       </c>
-      <c r="M114" s="2">
-        <f>61135-M113</f>
-        <v>46474</v>
+      <c r="M115" s="2">
+        <f>M114-M113</f>
+        <v>46214</v>
+      </c>
+      <c r="N115" s="2">
+        <f>61135-29997</f>
+        <v>31138</v>
+      </c>
+    </row>
+    <row r="118" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K118" t="s">
+        <v>145</v>
+      </c>
+      <c r="N118" s="2">
+        <v>16217</v>
+      </c>
+    </row>
+    <row r="119" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="N119" s="2">
+        <f>N118+M112</f>
+        <v>61135</v>
+      </c>
+    </row>
+    <row r="120" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="N120" s="2">
+        <f>N118+Table3[[#Totals],[Word Count]]</f>
+        <v>46214</v>
       </c>
     </row>
   </sheetData>
@@ -4052,10 +4098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E514ECA4-E30C-4BE7-995D-7555FADB58D2}">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5291,7 +5337,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C49">
         <f>22903-C48</f>
@@ -6190,10 +6236,18 @@
     </row>
     <row r="114" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F114" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H114" s="2">
-        <f>61135-H113</f>
+        <v>61135</v>
+      </c>
+    </row>
+    <row r="115" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
+        <v>146</v>
+      </c>
+      <c r="H115" s="2">
+        <f>H114-H113</f>
         <v>40581</v>
       </c>
     </row>

</xml_diff>